<commit_message>
Working on cleaning and commenting the code
</commit_message>
<xml_diff>
--- a/TOR330 Data/100x100trail/TOR330_2021.xlsx
+++ b/TOR330 Data/100x100trail/TOR330_2021.xlsx
@@ -2179,7 +2179,7 @@
     <t>Colle Franco</t>
   </si>
   <si>
-    <t>Jonas  Russi</t>
+    <t>Jonas Russi</t>
   </si>
   <si>
     <t>Restorp Petter</t>
@@ -2191,7 +2191,7 @@
     <t>Corsini Simone</t>
   </si>
   <si>
-    <t>Lucas  Jerome</t>
+    <t>Lucas Jerome</t>
   </si>
   <si>
     <t>Bosatelli Oliviero Ignazio</t>
@@ -2215,7 +2215,7 @@
     <t>Trigueros Garrote Silvia Ainhoa</t>
   </si>
   <si>
-    <t>Laving Jean-Marc</t>
+    <t>Laving Jean Marc</t>
   </si>
   <si>
     <t>Beaven Alexander</t>
@@ -2224,7 +2224,7 @@
     <t>Paganelli Melissa</t>
   </si>
   <si>
-    <t>Christin-Benoit Julien</t>
+    <t>Christin Benoit Julien</t>
   </si>
   <si>
     <t>Pulcini Giorgio</t>
@@ -2278,7 +2278,7 @@
     <t>Hewitt Michael</t>
   </si>
   <si>
-    <t>Jose Luis  Martinez Fernandez</t>
+    <t>Jose Luis Martinez Fernandez</t>
   </si>
   <si>
     <t>Orradre Inigo</t>
@@ -2287,7 +2287,7 @@
     <t>Vieira Nelson</t>
   </si>
   <si>
-    <t>Fernandez Canego  Angel</t>
+    <t>Fernandez Canego Angel</t>
   </si>
   <si>
     <t>Poskin Julien</t>
@@ -2305,7 +2305,7 @@
     <t>Hetmanski Adam</t>
   </si>
   <si>
-    <t>Pera Vall-Llosera Josep</t>
+    <t>Pera Vall Llosera Josep</t>
   </si>
   <si>
     <t>Carcano Miches</t>
@@ -2314,7 +2314,7 @@
     <t>Panaritis Panagiotis</t>
   </si>
   <si>
-    <t>Valsesia  Massimo</t>
+    <t>Valsesia Massimo</t>
   </si>
   <si>
     <t>Gregory Marrama</t>
@@ -2404,7 +2404,7 @@
     <t>Carrard Philippe</t>
   </si>
   <si>
-    <t>Jonathan  Soudy</t>
+    <t>Jonathan Soudy</t>
   </si>
   <si>
     <t>Broquet Xavier</t>
@@ -2413,7 +2413,7 @@
     <t>Forestieri Alexandre</t>
   </si>
   <si>
-    <t>Callisardi  Giancarlo</t>
+    <t>Callisardi Giancarlo</t>
   </si>
   <si>
     <t>Sebastien Pennazio</t>
@@ -2458,7 +2458,7 @@
     <t>Jongens Willemijn</t>
   </si>
   <si>
-    <t>Michaud Andre-Paul</t>
+    <t>Michaud Andre Paul</t>
   </si>
   <si>
     <t>Maccherini Tatiana</t>
@@ -2485,7 +2485,7 @@
     <t>Gravot Victor</t>
   </si>
   <si>
-    <t>Lucas-Frost Jonathan</t>
+    <t>Lucas Frost Jonathan</t>
   </si>
   <si>
     <t>Altmann Joachim</t>
@@ -2554,7 +2554,7 @@
     <t>Rossetti Nicoletta</t>
   </si>
   <si>
-    <t>Candido  Luca</t>
+    <t>Candido Luca</t>
   </si>
   <si>
     <t>Soares Miguel</t>
@@ -2698,7 +2698,7 @@
     <t>Rios Pita Ezequiel</t>
   </si>
   <si>
-    <t>Santamaria  Lorenzo</t>
+    <t>Santamaria Lorenzo</t>
   </si>
   <si>
     <t>Garcia Busto Eduardo</t>
@@ -2734,7 +2734,7 @@
     <t>Sciamanna Marco</t>
   </si>
   <si>
-    <t>Beretta  Roberto</t>
+    <t>Beretta Roberto</t>
   </si>
   <si>
     <t>Galassi Andrea</t>
@@ -2761,7 +2761,7 @@
     <t>Ducher Ludovic</t>
   </si>
   <si>
-    <t>Fortin Pierre-Luc</t>
+    <t>Fortin Pierre Luc</t>
   </si>
   <si>
     <t>Lafay Elodie</t>
@@ -3100,7 +3100,7 @@
     <t>Bassi Lorenzo</t>
   </si>
   <si>
-    <t>Patrick  Langelot</t>
+    <t>Patrick Langelot</t>
   </si>
   <si>
     <t>Buzzi Vittorio</t>
@@ -3112,7 +3112,7 @@
     <t>Hofer Florian</t>
   </si>
   <si>
-    <t>Jean-Yves Waty</t>
+    <t>Jean Yves Waty</t>
   </si>
   <si>
     <t>Colamartino Pietro</t>
@@ -3184,7 +3184,7 @@
     <t>Alves Henrique</t>
   </si>
   <si>
-    <t>Malo Jean-Yves</t>
+    <t>Malo Jean Yves</t>
   </si>
   <si>
     <t>Darnieaud Romain</t>
@@ -3196,7 +3196,7 @@
     <t>Ntikiadis Ioannis</t>
   </si>
   <si>
-    <t>Abbet Jean-Maurice</t>
+    <t>Abbet Jean Maurice</t>
   </si>
   <si>
     <t>Grangier Aline</t>
@@ -3208,7 +3208,7 @@
     <t>Baglione Marco</t>
   </si>
   <si>
-    <t>Reati  Alessandro</t>
+    <t>Reati Alessandro</t>
   </si>
   <si>
     <t>Underwood Tim</t>
@@ -3232,7 +3232,7 @@
     <t>Watteyne Martin</t>
   </si>
   <si>
-    <t>Veyre  Aurelia</t>
+    <t>Veyre Aurelia</t>
   </si>
   <si>
     <t>Mayer Doug</t>
@@ -3250,7 +3250,7 @@
     <t>Massalin Andrea</t>
   </si>
   <si>
-    <t>Zanella  Thierry</t>
+    <t>Zanella Thierry</t>
   </si>
   <si>
     <t>Lassus Emmanuel</t>
@@ -3262,7 +3262,7 @@
     <t>Jegu Corentin</t>
   </si>
   <si>
-    <t>Cavallari  Cristian</t>
+    <t>Cavallari Cristian</t>
   </si>
   <si>
     <t>Fornasier Fausto</t>
@@ -3319,7 +3319,7 @@
     <t>Bianchi Federico</t>
   </si>
   <si>
-    <t>Castillo Carrascal  Paco</t>
+    <t>Castillo Carrascal Paco</t>
   </si>
   <si>
     <t>Abbet Valentin</t>
@@ -3352,7 +3352,7 @@
     <t>Garelli Giorgio</t>
   </si>
   <si>
-    <t>Nicaise Jean-Baptiste</t>
+    <t>Nicaise Jean Baptiste</t>
   </si>
   <si>
     <t>Reichardt Frank</t>
@@ -3373,7 +3373,7 @@
     <t>Hidalgo Vasco Javier</t>
   </si>
   <si>
-    <t>Carmona Marina Jose  Fernando</t>
+    <t>Carmona Marina Jose Fernando</t>
   </si>
   <si>
     <t>Billi Francesca</t>
@@ -3481,7 +3481,7 @@
     <t>Sweeris Esther</t>
   </si>
   <si>
-    <t>Barbara  Plovier</t>
+    <t>Barbara Plovier</t>
   </si>
   <si>
     <t>Marques Valerie</t>
@@ -3643,13 +3643,13 @@
     <t>Santi Amantini Valentino</t>
   </si>
   <si>
-    <t>Louis-Jacquet Olivier</t>
+    <t>Louis Jacquet Olivier</t>
   </si>
   <si>
     <t>Simonotti Marco</t>
   </si>
   <si>
-    <t>Chudy  Przemyslaw</t>
+    <t>Chudy Przemyslaw</t>
   </si>
   <si>
     <t>Felicite Gilles</t>
@@ -3670,7 +3670,7 @@
     <t>Cheal Mark</t>
   </si>
   <si>
-    <t>Le Floch Jean-Pascal</t>
+    <t>Le Floch Jean Pascal</t>
   </si>
   <si>
     <t>Zavelani Rossi Maria Beatrice</t>
@@ -3688,7 +3688,7 @@
     <t>Suwannachairop Sukthawee</t>
   </si>
   <si>
-    <t>Usanawasin  Sakuna</t>
+    <t>Usanawasin Sakuna</t>
   </si>
   <si>
     <t>Ferri Giorgio</t>
@@ -3706,7 +3706,7 @@
     <t>Errico Domenico</t>
   </si>
   <si>
-    <t>Meyer Jean-Francois</t>
+    <t>Meyer Jean Francois</t>
   </si>
   <si>
     <t>Canton Annalisa</t>
@@ -3892,7 +3892,7 @@
     <t>Reynolds Galen</t>
   </si>
   <si>
-    <t>Schmidt  Michael</t>
+    <t>Schmidt Michael</t>
   </si>
   <si>
     <t>Cambriglia Luca</t>
@@ -3901,7 +3901,7 @@
     <t>Benoit Clement</t>
   </si>
   <si>
-    <t>Lavie Jean-Marc</t>
+    <t>Lavie Jean Marc</t>
   </si>
   <si>
     <t>Jerome Marin</t>
@@ -4099,7 +4099,7 @@
     <t>Grenti Filippo</t>
   </si>
   <si>
-    <t>Portemer  Sebastien</t>
+    <t>Portemer Sebastien</t>
   </si>
   <si>
     <t>Drouet Thierry</t>
@@ -4165,7 +4165,7 @@
     <t>Dominique Di Vincenzo</t>
   </si>
   <si>
-    <t>Jean-Philippe Compan</t>
+    <t>Jean Philippe Compan</t>
   </si>
   <si>
     <t>Calcagni Donato Antonio</t>
@@ -4183,7 +4183,7 @@
     <t>Iannone Alessandro</t>
   </si>
   <si>
-    <t>Gazzaniga  Andrea</t>
+    <t>Gazzaniga Andrea</t>
   </si>
   <si>
     <t>Fugante Massimo</t>
@@ -4291,7 +4291,7 @@
     <t>Roukema Arjan</t>
   </si>
   <si>
-    <t>Bosser Jean-Luc</t>
+    <t>Bosser Jean Luc</t>
   </si>
   <si>
     <t>Sampaio Joaquim</t>
@@ -4300,7 +4300,7 @@
     <t>Jourdan Mikael</t>
   </si>
   <si>
-    <t>Marziano  Gianfranco</t>
+    <t>Marziano Gianfranco</t>
   </si>
   <si>
     <t>Dohrmann Michael</t>

</xml_diff>